<commit_message>
feat(karma_voucher): add base-template api
</commit_message>
<xml_diff>
--- a/api/dashboard/karma_voucher/assets/base_template.xlsx
+++ b/api/dashboard/karma_voucher/assets/base_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2 mulearn\mulearnbackend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerom\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC84E8A-D929-4EE8-92BA-46477F27296D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C151EA74-02B6-4CF1-B2CB-529DF1945789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,7 +428,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -437,7 +437,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
refactor(karma_voucher): base template api
</commit_message>
<xml_diff>
--- a/api/dashboard/karma_voucher/assets/base_template.xlsx
+++ b/api/dashboard/karma_voucher/assets/base_template.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerom\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2 mulearn\mulearnbackend\api\dashboard\karma_voucher\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C151EA74-02B6-4CF1-B2CB-529DF1945789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C26FF8-F408-4778-824B-F3B296751D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Data Defenitions" sheetId="2" r:id="rId2"/>
+    <sheet name="Data Definitions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>

</xml_diff>